<commit_message>
updated draft order and needs - march 23
</commit_message>
<xml_diff>
--- a/top_200_players.xlsx
+++ b/top_200_players.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\UALR\Artificial Intelligence\final project\borromeoz-ai-final\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\UALR\Artificial Intelligence\borromeoz-mock-draft\NFL-Mock-Draft\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C3C0BB5-5A0C-4F83-B798-471CBB840B5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A915E425-2831-4020-A6F8-E2BB86537C3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{AAF647CF-EBD0-4CEE-B90A-ABDDD2056A3C}"/>
   </bookViews>
@@ -3194,7 +3194,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18EDEC17-FB3B-4270-98E8-171D112580F2}">
   <dimension ref="A1:L290"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A226" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B244" sqref="B244"/>
     </sheetView>
   </sheetViews>

</xml_diff>